<commit_message>
Update achievement, exam questions.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A561C0A-8FF0-4980-83C5-8D0FF522C7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3AC1E0-2C5E-41E1-94C8-C11055971542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,27 +581,27 @@
   <dimension ref="A1:AL999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" customWidth="1"/>
-    <col min="4" max="12" width="5.109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="5.21875" customWidth="1"/>
-    <col min="14" max="22" width="5.109375" customWidth="1"/>
-    <col min="23" max="23" width="4.88671875" customWidth="1"/>
-    <col min="24" max="28" width="5.109375" customWidth="1"/>
-    <col min="29" max="30" width="4.88671875" customWidth="1"/>
-    <col min="31" max="31" width="6.33203125" customWidth="1"/>
-    <col min="32" max="32" width="7" customWidth="1"/>
-    <col min="33" max="33" width="6.5546875" customWidth="1"/>
-    <col min="34" max="34" width="15" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" hidden="1" customWidth="1"/>
+    <col min="4" max="11" width="4.77734375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="6.109375" customWidth="1"/>
+    <col min="14" max="15" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="30" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9" customWidth="1"/>
-    <col min="36" max="36" width="10" customWidth="1"/>
-    <col min="37" max="37" width="7.6640625" customWidth="1"/>
+    <col min="36" max="36" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -738,8 +738,12 @@
         <v>0</v>
       </c>
       <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="N2" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0.75</v>
+      </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -757,30 +761,30 @@
       <c r="AD2" s="1"/>
       <c r="AE2" s="1">
         <f t="shared" ref="AE2:AE43" si="1">SUM(M2:AD2)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AF2" s="1">
         <f t="shared" ref="AF2:AF43" si="2">L2+AE2</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AG2" s="1">
         <f t="shared" ref="AG2:AG42" si="3">AG3</f>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH2" s="3">
         <f t="shared" ref="AH2:AH43" si="4">(AF2/AG2)*100</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AI2" s="3">
         <f t="shared" ref="AI2:AI43" si="5">MAX(IF(AH2&gt;=20,2,0),IF(AH2&gt;=40,3,0),IF(AH2&gt;=60,4,0),IF(AH2&gt;=80,5,0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ2" s="3">
         <v>0</v>
       </c>
       <c r="AK2" s="3">
         <f>0.8*AI2+0.2*AJ2</f>
-        <v>0</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="AL2" s="4"/>
     </row>
@@ -803,8 +807,12 @@
         <v>0</v>
       </c>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+      <c r="N3" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.75</v>
+      </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -822,30 +830,30 @@
       <c r="AD3" s="1"/>
       <c r="AE3" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF3" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG3" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH3" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="AI3" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AJ3" s="3">
         <v>0</v>
       </c>
       <c r="AK3" s="10">
         <f t="shared" ref="AK3:AK43" si="6">0.8*AI3+0.2*AJ3</f>
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="AL3" s="4"/>
     </row>
@@ -895,7 +903,7 @@
       </c>
       <c r="AG4" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH4" s="3">
         <f t="shared" si="4"/>
@@ -934,7 +942,9 @@
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="1"/>
@@ -960,7 +970,7 @@
       </c>
       <c r="AG5" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH5" s="3">
         <f t="shared" si="4"/>
@@ -1000,8 +1010,12 @@
         <v>0</v>
       </c>
       <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="1"/>
@@ -1019,30 +1033,30 @@
       <c r="AD6" s="1"/>
       <c r="AE6" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF6" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH6" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AI6" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ6" s="3">
         <v>0</v>
       </c>
       <c r="AK6" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AL6" s="4"/>
     </row>
@@ -1065,8 +1079,12 @@
         <v>0</v>
       </c>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="1"/>
@@ -1092,7 +1110,7 @@
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH7" s="3">
         <f t="shared" si="4"/>
@@ -1157,7 +1175,7 @@
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH8" s="3">
         <f t="shared" si="4"/>
@@ -1195,7 +1213,9 @@
         <v>0</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="6"/>
@@ -1222,7 +1242,7 @@
       </c>
       <c r="AG9" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH9" s="3">
         <f t="shared" si="4"/>
@@ -1260,8 +1280,12 @@
         <v>0</v>
       </c>
       <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="1"/>
@@ -1287,7 +1311,7 @@
       </c>
       <c r="AG10" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH10" s="3">
         <f t="shared" si="4"/>
@@ -1352,7 +1376,7 @@
       </c>
       <c r="AG11" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH11" s="3">
         <f t="shared" si="4"/>
@@ -1417,7 +1441,7 @@
       </c>
       <c r="AG12" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH12" s="3">
         <f t="shared" si="4"/>
@@ -1455,7 +1479,9 @@
         <v>0</v>
       </c>
       <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="6"/>
@@ -1482,7 +1508,7 @@
       </c>
       <c r="AG13" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH13" s="3">
         <f t="shared" si="4"/>
@@ -1520,7 +1546,9 @@
         <v>0</v>
       </c>
       <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="N14" s="1">
+        <v>0.5</v>
+      </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="6"/>
@@ -1539,19 +1567,19 @@
       <c r="AD14" s="1"/>
       <c r="AE14" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AF14" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AG14" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH14" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="AI14" s="3">
         <f t="shared" si="5"/>
@@ -1586,7 +1614,9 @@
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
+      <c r="O15" s="1">
+        <v>1</v>
+      </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -1604,30 +1634,30 @@
       <c r="AD15" s="1"/>
       <c r="AE15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF15" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG15" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH15" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AI15" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ15" s="3">
         <v>0</v>
       </c>
       <c r="AK15" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AL15" s="4"/>
     </row>
@@ -1677,7 +1707,7 @@
       </c>
       <c r="AG16" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH16" s="3">
         <f t="shared" si="4"/>
@@ -1742,7 +1772,7 @@
       </c>
       <c r="AG17" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH17" s="3">
         <f t="shared" si="4"/>
@@ -1780,8 +1810,12 @@
         <v>0</v>
       </c>
       <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>1</v>
+      </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="1"/>
@@ -1799,30 +1833,30 @@
       <c r="AD18" s="1"/>
       <c r="AE18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF18" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG18" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH18" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AI18" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ18" s="3">
         <v>0</v>
       </c>
       <c r="AK18" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AL18" s="4"/>
     </row>
@@ -1872,7 +1906,7 @@
       </c>
       <c r="AG19" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH19" s="3">
         <f t="shared" si="4"/>
@@ -1937,7 +1971,7 @@
       </c>
       <c r="AG20" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH20" s="3">
         <f t="shared" si="4"/>
@@ -1975,7 +2009,9 @@
         <v>0</v>
       </c>
       <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="7"/>
@@ -2002,7 +2038,7 @@
       </c>
       <c r="AG21" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH21" s="3">
         <f t="shared" si="4"/>
@@ -2067,7 +2103,7 @@
       </c>
       <c r="AG22" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH22" s="3">
         <f t="shared" si="4"/>
@@ -2132,7 +2168,7 @@
       </c>
       <c r="AG23" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH23" s="3">
         <f t="shared" si="4"/>
@@ -2197,7 +2233,7 @@
       </c>
       <c r="AG24" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH24" s="3">
         <f t="shared" si="4"/>
@@ -2264,7 +2300,7 @@
       </c>
       <c r="AG25" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH25" s="3">
         <f t="shared" si="4"/>
@@ -2302,7 +2338,9 @@
         <v>0</v>
       </c>
       <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="7"/>
@@ -2329,7 +2367,7 @@
       </c>
       <c r="AG26" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH26" s="3">
         <f t="shared" si="4"/>
@@ -2394,7 +2432,7 @@
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH27" s="3">
         <f t="shared" si="4"/>
@@ -2459,7 +2497,7 @@
       </c>
       <c r="AG28" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH28" s="3">
         <f t="shared" si="4"/>
@@ -2524,7 +2562,7 @@
       </c>
       <c r="AG29" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH29" s="3">
         <f t="shared" si="4"/>
@@ -2589,7 +2627,7 @@
       </c>
       <c r="AG30" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH30" s="3">
         <f t="shared" si="4"/>
@@ -2654,7 +2692,7 @@
       </c>
       <c r="AG31" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH31" s="3">
         <f t="shared" si="4"/>
@@ -2719,7 +2757,7 @@
       </c>
       <c r="AG32" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH32" s="3">
         <f t="shared" si="4"/>
@@ -2784,7 +2822,7 @@
       </c>
       <c r="AG33" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH33" s="3">
         <f t="shared" si="4"/>
@@ -2849,7 +2887,7 @@
       </c>
       <c r="AG34" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH34" s="3">
         <f t="shared" si="4"/>
@@ -2914,7 +2952,7 @@
       </c>
       <c r="AG35" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH35" s="3">
         <f t="shared" si="4"/>
@@ -2979,7 +3017,7 @@
       </c>
       <c r="AG36" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH36" s="3">
         <f t="shared" si="4"/>
@@ -3044,7 +3082,7 @@
       </c>
       <c r="AG37" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH37" s="3">
         <f t="shared" si="4"/>
@@ -3109,7 +3147,7 @@
       </c>
       <c r="AG38" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH38" s="3">
         <f t="shared" si="4"/>
@@ -3174,7 +3212,7 @@
       </c>
       <c r="AG39" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH39" s="3">
         <f t="shared" si="4"/>
@@ -3239,7 +3277,7 @@
       </c>
       <c r="AG40" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH40" s="3">
         <f t="shared" si="4"/>
@@ -3304,7 +3342,7 @@
       </c>
       <c r="AG41" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH41" s="3">
         <f t="shared" si="4"/>
@@ -3369,7 +3407,7 @@
       </c>
       <c r="AG42" s="1">
         <f t="shared" si="3"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH42" s="3">
         <f t="shared" si="4"/>
@@ -3413,62 +3451,32 @@
       <c r="O43" s="1">
         <v>1.5</v>
       </c>
-      <c r="P43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="Q43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="R43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="S43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="T43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="U43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="V43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="W43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="X43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="Y43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="Z43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="AA43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="AB43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="AC43" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="AD43" s="1">
-        <v>1.5</v>
-      </c>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1"/>
+      <c r="AB43" s="1"/>
+      <c r="AC43" s="1"/>
+      <c r="AD43" s="1"/>
       <c r="AE43" s="1">
         <f t="shared" si="1"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AF43" s="1">
         <f t="shared" si="2"/>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AG43" s="1">
         <f>AF43</f>
-        <v>25.5</v>
+        <v>3</v>
       </c>
       <c r="AH43" s="3">
         <f t="shared" si="4"/>
@@ -41729,6 +41737,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update achievement, tasks. Add 12, 13 lectures.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3AC1E0-2C5E-41E1-94C8-C11055971542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440F1D16-8E0E-4263-89DC-51FCC150FB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:AL999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -591,10 +591,10 @@
     <col min="3" max="3" width="4.44140625" hidden="1" customWidth="1"/>
     <col min="4" max="11" width="4.77734375" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="2.6640625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="6.109375" customWidth="1"/>
+    <col min="13" max="13" width="2.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="21" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="30" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.44140625" customWidth="1"/>
+    <col min="17" max="30" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="6" bestFit="1" customWidth="1"/>
@@ -769,22 +769,22 @@
       </c>
       <c r="AG2" s="1">
         <f t="shared" ref="AG2:AG42" si="3">AG3</f>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH2" s="3">
         <f t="shared" ref="AH2:AH43" si="4">(AF2/AG2)*100</f>
-        <v>50</v>
+        <v>5.8823529411764701</v>
       </c>
       <c r="AI2" s="3">
         <f t="shared" ref="AI2:AI43" si="5">MAX(IF(AH2&gt;=20,2,0),IF(AH2&gt;=40,3,0),IF(AH2&gt;=60,4,0),IF(AH2&gt;=80,5,0))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ2" s="3">
         <v>0</v>
       </c>
       <c r="AK2" s="3">
         <f>0.8*AI2+0.2*AJ2</f>
-        <v>2.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="AL2" s="4"/>
     </row>
@@ -838,22 +838,22 @@
       </c>
       <c r="AG3" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH3" s="3">
         <f t="shared" si="4"/>
-        <v>66.666666666666657</v>
+        <v>7.8431372549019605</v>
       </c>
       <c r="AI3" s="3">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AJ3" s="3">
         <v>0</v>
       </c>
       <c r="AK3" s="10">
         <f t="shared" ref="AK3:AK43" si="6">0.8*AI3+0.2*AJ3</f>
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="AL3" s="4"/>
     </row>
@@ -903,7 +903,7 @@
       </c>
       <c r="AG4" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH4" s="3">
         <f t="shared" si="4"/>
@@ -945,7 +945,9 @@
       <c r="O5" s="1">
         <v>0</v>
       </c>
-      <c r="P5" s="1"/>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
       <c r="Q5" s="7"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -970,7 +972,7 @@
       </c>
       <c r="AG5" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH5" s="3">
         <f t="shared" si="4"/>
@@ -1041,22 +1043,22 @@
       </c>
       <c r="AG6" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH6" s="3">
         <f t="shared" si="4"/>
-        <v>33.333333333333329</v>
+        <v>3.9215686274509802</v>
       </c>
       <c r="AI6" s="3">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ6" s="3">
         <v>0</v>
       </c>
       <c r="AK6" s="10">
         <f t="shared" si="6"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="AL6" s="4"/>
     </row>
@@ -1110,7 +1112,7 @@
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH7" s="3">
         <f t="shared" si="4"/>
@@ -1175,7 +1177,7 @@
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH8" s="3">
         <f t="shared" si="4"/>
@@ -1216,8 +1218,12 @@
       <c r="N9" s="1">
         <v>0</v>
       </c>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>2</v>
+      </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -1234,19 +1240,19 @@
       <c r="AD9" s="1"/>
       <c r="AE9" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF9" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG9" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH9" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7.8431372549019605</v>
       </c>
       <c r="AI9" s="3">
         <f t="shared" si="5"/>
@@ -1311,7 +1317,7 @@
       </c>
       <c r="AG10" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH10" s="3">
         <f t="shared" si="4"/>
@@ -1376,7 +1382,7 @@
       </c>
       <c r="AG11" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH11" s="3">
         <f t="shared" si="4"/>
@@ -1441,7 +1447,7 @@
       </c>
       <c r="AG12" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH12" s="3">
         <f t="shared" si="4"/>
@@ -1482,8 +1488,12 @@
       <c r="N13" s="1">
         <v>0</v>
       </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0.75</v>
+      </c>
       <c r="Q13" s="6"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -1500,19 +1510,19 @@
       <c r="AD13" s="1"/>
       <c r="AE13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AF13" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AG13" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH13" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.9411764705882351</v>
       </c>
       <c r="AI13" s="3">
         <f t="shared" si="5"/>
@@ -1575,11 +1585,11 @@
       </c>
       <c r="AG14" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH14" s="3">
         <f t="shared" si="4"/>
-        <v>16.666666666666664</v>
+        <v>1.9607843137254901</v>
       </c>
       <c r="AI14" s="3">
         <f t="shared" si="5"/>
@@ -1642,22 +1652,22 @@
       </c>
       <c r="AG15" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH15" s="3">
         <f t="shared" si="4"/>
-        <v>33.333333333333329</v>
+        <v>3.9215686274509802</v>
       </c>
       <c r="AI15" s="3">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ15" s="3">
         <v>0</v>
       </c>
       <c r="AK15" s="10">
         <f t="shared" si="6"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="AL15" s="4"/>
     </row>
@@ -1707,7 +1717,7 @@
       </c>
       <c r="AG16" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH16" s="3">
         <f t="shared" si="4"/>
@@ -1772,7 +1782,7 @@
       </c>
       <c r="AG17" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH17" s="3">
         <f t="shared" si="4"/>
@@ -1841,22 +1851,22 @@
       </c>
       <c r="AG18" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH18" s="3">
         <f t="shared" si="4"/>
-        <v>33.333333333333329</v>
+        <v>3.9215686274509802</v>
       </c>
       <c r="AI18" s="3">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ18" s="3">
         <v>0</v>
       </c>
       <c r="AK18" s="10">
         <f t="shared" si="6"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="AL18" s="4"/>
     </row>
@@ -1906,7 +1916,7 @@
       </c>
       <c r="AG19" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH19" s="3">
         <f t="shared" si="4"/>
@@ -1971,7 +1981,7 @@
       </c>
       <c r="AG20" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH20" s="3">
         <f t="shared" si="4"/>
@@ -2038,7 +2048,7 @@
       </c>
       <c r="AG21" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH21" s="3">
         <f t="shared" si="4"/>
@@ -2103,7 +2113,7 @@
       </c>
       <c r="AG22" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH22" s="3">
         <f t="shared" si="4"/>
@@ -2168,7 +2178,7 @@
       </c>
       <c r="AG23" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH23" s="3">
         <f t="shared" si="4"/>
@@ -2233,7 +2243,7 @@
       </c>
       <c r="AG24" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH24" s="3">
         <f t="shared" si="4"/>
@@ -2300,7 +2310,7 @@
       </c>
       <c r="AG25" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH25" s="3">
         <f t="shared" si="4"/>
@@ -2367,7 +2377,7 @@
       </c>
       <c r="AG26" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH26" s="3">
         <f t="shared" si="4"/>
@@ -2432,7 +2442,7 @@
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH27" s="3">
         <f t="shared" si="4"/>
@@ -2497,7 +2507,7 @@
       </c>
       <c r="AG28" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH28" s="3">
         <f t="shared" si="4"/>
@@ -2562,7 +2572,7 @@
       </c>
       <c r="AG29" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH29" s="3">
         <f t="shared" si="4"/>
@@ -2627,7 +2637,7 @@
       </c>
       <c r="AG30" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH30" s="3">
         <f t="shared" si="4"/>
@@ -2692,7 +2702,7 @@
       </c>
       <c r="AG31" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH31" s="3">
         <f t="shared" si="4"/>
@@ -2757,7 +2767,7 @@
       </c>
       <c r="AG32" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH32" s="3">
         <f t="shared" si="4"/>
@@ -2822,7 +2832,7 @@
       </c>
       <c r="AG33" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH33" s="3">
         <f t="shared" si="4"/>
@@ -2887,7 +2897,7 @@
       </c>
       <c r="AG34" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH34" s="3">
         <f t="shared" si="4"/>
@@ -2952,7 +2962,7 @@
       </c>
       <c r="AG35" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH35" s="3">
         <f t="shared" si="4"/>
@@ -3017,7 +3027,7 @@
       </c>
       <c r="AG36" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH36" s="3">
         <f t="shared" si="4"/>
@@ -3082,7 +3092,7 @@
       </c>
       <c r="AG37" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH37" s="3">
         <f t="shared" si="4"/>
@@ -3147,7 +3157,7 @@
       </c>
       <c r="AG38" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH38" s="3">
         <f t="shared" si="4"/>
@@ -3212,7 +3222,7 @@
       </c>
       <c r="AG39" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH39" s="3">
         <f t="shared" si="4"/>
@@ -3277,7 +3287,7 @@
       </c>
       <c r="AG40" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH40" s="3">
         <f t="shared" si="4"/>
@@ -3342,7 +3352,7 @@
       </c>
       <c r="AG41" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH41" s="3">
         <f t="shared" si="4"/>
@@ -3407,7 +3417,7 @@
       </c>
       <c r="AG42" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH42" s="3">
         <f t="shared" si="4"/>
@@ -3451,32 +3461,62 @@
       <c r="O43" s="1">
         <v>1.5</v>
       </c>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
-      <c r="X43" s="1"/>
-      <c r="Y43" s="1"/>
-      <c r="Z43" s="1"/>
-      <c r="AA43" s="1"/>
-      <c r="AB43" s="1"/>
-      <c r="AC43" s="1"/>
-      <c r="AD43" s="1"/>
+      <c r="P43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="R43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="S43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="T43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="U43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="V43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="W43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="X43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Y43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Z43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AA43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AB43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AC43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AD43" s="1">
+        <v>1.5</v>
+      </c>
       <c r="AE43" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AF43" s="1">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AG43" s="1">
         <f>AF43</f>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="AH43" s="3">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
Update achievement, tasks. Add 14 - 19 lectures.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4997C220-D948-49B5-83D3-3F4BBA89BCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6E4D69-82DC-4D1B-B800-65C4FA426B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,7 +365,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -594,7 +594,7 @@
     <col min="13" max="13" width="2.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5.44140625" customWidth="1"/>
-    <col min="17" max="17" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="19" max="30" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="5.44140625" bestFit="1" customWidth="1"/>
@@ -724,7 +724,7 @@
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -736,12 +736,12 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1">
-        <f t="shared" ref="L2:L43" si="0">SUM(C2:K2)</f>
+        <f t="shared" ref="L2:L42" si="0">SUM(C2:K2)</f>
         <v>0</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="O2" s="1">
         <v>0.75</v>
@@ -762,30 +762,30 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
       <c r="AE2" s="1">
-        <f t="shared" ref="AE2:AE43" si="1">SUM(M2:AD2)</f>
-        <v>1.5</v>
+        <f t="shared" ref="AE2:AE42" si="1">SUM(M2:AD2)</f>
+        <v>2</v>
       </c>
       <c r="AF2" s="1">
-        <f t="shared" ref="AF2:AF43" si="2">L2+AE2</f>
-        <v>1.5</v>
+        <f t="shared" ref="AF2:AF42" si="2">L2+AE2</f>
+        <v>2</v>
       </c>
       <c r="AG2" s="1">
         <f t="shared" ref="AG2:AG42" si="3">AG3</f>
         <v>25.5</v>
       </c>
       <c r="AH2" s="3">
-        <f t="shared" ref="AH2:AH43" si="4">(AF2/AG2)*100</f>
-        <v>5.8823529411764701</v>
+        <f t="shared" ref="AH2:AH42" si="4">(AF2/AG2)*100</f>
+        <v>7.8431372549019605</v>
       </c>
       <c r="AI2" s="3">
-        <f t="shared" ref="AI2:AI43" si="5">MAX(IF(AH2&gt;=20,2,0),IF(AH2&gt;=40,3,0),IF(AH2&gt;=60,4,0),IF(AH2&gt;=80,5,0))</f>
+        <f t="shared" ref="AI2:AI42" si="5">MAX(IF(AH2&gt;=20,2,0),IF(AH2&gt;=40,3,0),IF(AH2&gt;=60,4,0),IF(AH2&gt;=80,5,0))</f>
         <v>0</v>
       </c>
       <c r="AJ2" s="3">
         <v>0</v>
       </c>
       <c r="AK2" s="3">
-        <f>0.8*AI2+0.2*AJ2</f>
+        <f t="shared" ref="AK2:AK42" si="6">0.8*AI2+0.2*AJ2</f>
         <v>0</v>
       </c>
       <c r="AL2" s="4"/>
@@ -793,7 +793,7 @@
     <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -810,13 +810,15 @@
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="O3" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="7"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -854,7 +856,7 @@
         <v>0</v>
       </c>
       <c r="AK3" s="10">
-        <f t="shared" ref="AK3:AK43" si="6">0.8*AI3+0.2*AJ3</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AL3" s="4"/>
@@ -862,7 +864,7 @@
     <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -878,12 +880,18 @@
         <v>0</v>
       </c>
       <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.75</v>
+      </c>
       <c r="Q4" s="6"/>
       <c r="R4" s="1">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -899,11 +907,11 @@
       <c r="AD4" s="1"/>
       <c r="AE4" s="1">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="AF4" s="1">
         <f t="shared" si="2"/>
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="AG4" s="1">
         <f t="shared" si="3"/>
@@ -911,7 +919,7 @@
       </c>
       <c r="AH4" s="3">
         <f t="shared" si="4"/>
-        <v>2.9411764705882351</v>
+        <v>7.8431372549019605</v>
       </c>
       <c r="AI4" s="3">
         <f t="shared" si="5"/>
@@ -929,7 +937,7 @@
     <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -947,12 +955,12 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1">
+        <v>1</v>
+      </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -968,11 +976,11 @@
       <c r="AD5" s="1"/>
       <c r="AE5" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF5" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG5" s="1">
         <f t="shared" si="3"/>
@@ -980,7 +988,7 @@
       </c>
       <c r="AH5" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7.8431372549019605</v>
       </c>
       <c r="AI5" s="3">
         <f t="shared" si="5"/>
@@ -996,11 +1004,9 @@
       <c r="AL5" s="4"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1017,14 +1023,16 @@
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1">
-        <v>1</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="1"/>
+      <c r="Q6" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0.5</v>
+      </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -1039,11 +1047,11 @@
       <c r="AD6" s="1"/>
       <c r="AE6" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="AF6" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="AG6" s="1">
         <f t="shared" si="3"/>
@@ -1051,7 +1059,7 @@
       </c>
       <c r="AH6" s="3">
         <f t="shared" si="4"/>
-        <v>3.9215686274509802</v>
+        <v>6.8627450980392162</v>
       </c>
       <c r="AI6" s="3">
         <f t="shared" si="5"/>
@@ -1069,7 +1077,7 @@
     <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1086,15 +1094,13 @@
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="O7" s="1">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="Q7" s="6">
-        <v>1</v>
-      </c>
+      <c r="Q7" s="8"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -1110,11 +1116,11 @@
       <c r="AD7" s="1"/>
       <c r="AE7" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AF7" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="3"/>
@@ -1122,7 +1128,7 @@
       </c>
       <c r="AH7" s="3">
         <f t="shared" si="4"/>
-        <v>3.9215686274509802</v>
+        <v>5.8823529411764701</v>
       </c>
       <c r="AI7" s="3">
         <f t="shared" si="5"/>
@@ -1138,9 +1144,11 @@
       <c r="AL7" s="4"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1156,10 +1164,14 @@
         <v>0</v>
       </c>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="N8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
       <c r="P8" s="1"/>
-      <c r="Q8" s="7"/>
+      <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -1175,11 +1187,11 @@
       <c r="AD8" s="1"/>
       <c r="AE8" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF8" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="3"/>
@@ -1187,7 +1199,7 @@
       </c>
       <c r="AH8" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.9215686274509802</v>
       </c>
       <c r="AI8" s="3">
         <f t="shared" si="5"/>
@@ -1205,7 +1217,7 @@
     <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1227,10 +1239,10 @@
       <c r="O9" s="1">
         <v>0</v>
       </c>
-      <c r="P9" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="6"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="6">
+        <v>1</v>
+      </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -1246,11 +1258,11 @@
       <c r="AD9" s="1"/>
       <c r="AE9" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF9" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG9" s="1">
         <f t="shared" si="3"/>
@@ -1258,7 +1270,7 @@
       </c>
       <c r="AH9" s="3">
         <f t="shared" si="4"/>
-        <v>7.8431372549019605</v>
+        <v>3.9215686274509802</v>
       </c>
       <c r="AI9" s="3">
         <f t="shared" si="5"/>
@@ -1276,7 +1288,7 @@
     <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="5" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1296,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="6"/>
@@ -1315,11 +1327,11 @@
       <c r="AD10" s="1"/>
       <c r="AE10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF10" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10" s="1">
         <f t="shared" si="3"/>
@@ -1327,7 +1339,7 @@
       </c>
       <c r="AH10" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.9215686274509802</v>
       </c>
       <c r="AI10" s="3">
         <f t="shared" si="5"/>
@@ -1345,7 +1357,7 @@
     <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1365,7 +1377,9 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="7"/>
-      <c r="R11" s="1"/>
+      <c r="R11" s="1">
+        <v>0.75</v>
+      </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -1380,11 +1394,11 @@
       <c r="AD11" s="1"/>
       <c r="AE11" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AF11" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AG11" s="1">
         <f t="shared" si="3"/>
@@ -1392,7 +1406,7 @@
       </c>
       <c r="AH11" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.9411764705882351</v>
       </c>
       <c r="AI11" s="3">
         <f t="shared" si="5"/>
@@ -1408,9 +1422,11 @@
       <c r="AL11" s="4"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B12" s="5" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1429,8 +1445,10 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1">
+        <v>0.5</v>
+      </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
@@ -1445,11 +1463,11 @@
       <c r="AD12" s="1"/>
       <c r="AE12" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AF12" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AG12" s="1">
         <f t="shared" si="3"/>
@@ -1457,7 +1475,7 @@
       </c>
       <c r="AH12" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.9607843137254901</v>
       </c>
       <c r="AI12" s="3">
         <f t="shared" si="5"/>
@@ -1475,7 +1493,7 @@
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1494,15 +1512,11 @@
       <c r="N13" s="1">
         <v>0</v>
       </c>
-      <c r="O13" s="1">
-        <v>0</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0.75</v>
-      </c>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="1">
-        <v>1.25</v>
+        <v>0.5</v>
       </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -1518,11 +1532,11 @@
       <c r="AD13" s="1"/>
       <c r="AE13" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AF13" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AG13" s="1">
         <f t="shared" si="3"/>
@@ -1530,7 +1544,7 @@
       </c>
       <c r="AH13" s="3">
         <f t="shared" si="4"/>
-        <v>7.8431372549019605</v>
+        <v>1.9607843137254901</v>
       </c>
       <c r="AI13" s="3">
         <f t="shared" si="5"/>
@@ -1548,7 +1562,7 @@
     <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1564,15 +1578,15 @@
         <v>0</v>
       </c>
       <c r="M14" s="1"/>
-      <c r="N14" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
       <c r="Q14" s="6"/>
-      <c r="R14" s="1">
-        <v>0.75</v>
-      </c>
+      <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
@@ -1587,11 +1601,11 @@
       <c r="AD14" s="1"/>
       <c r="AE14" s="1">
         <f t="shared" si="1"/>
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="AF14" s="1">
         <f t="shared" si="2"/>
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="AG14" s="1">
         <f t="shared" si="3"/>
@@ -1599,7 +1613,7 @@
       </c>
       <c r="AH14" s="3">
         <f t="shared" si="4"/>
-        <v>4.9019607843137258</v>
+        <v>0</v>
       </c>
       <c r="AI14" s="3">
         <f t="shared" si="5"/>
@@ -1617,7 +1631,7 @@
     <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1634,15 +1648,13 @@
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="1">
-        <v>1</v>
-      </c>
+      <c r="O15" s="1"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="1">
-        <v>1</v>
-      </c>
+      <c r="Q15" s="7"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
+      <c r="S15" s="1">
+        <v>0.5</v>
+      </c>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
@@ -1656,11 +1668,11 @@
       <c r="AD15" s="1"/>
       <c r="AE15" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AF15" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AG15" s="1">
         <f t="shared" si="3"/>
@@ -1668,7 +1680,7 @@
       </c>
       <c r="AH15" s="3">
         <f t="shared" si="4"/>
-        <v>7.8431372549019605</v>
+        <v>1.9607843137254901</v>
       </c>
       <c r="AI15" s="3">
         <f t="shared" si="5"/>
@@ -1686,7 +1698,7 @@
     <row r="16" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1702,12 +1714,18 @@
         <v>0</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0</v>
+      </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
+      <c r="S16" s="1">
+        <v>1</v>
+      </c>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
@@ -1721,11 +1739,11 @@
       <c r="AD16" s="1"/>
       <c r="AE16" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF16" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG16" s="1">
         <f t="shared" si="3"/>
@@ -1733,7 +1751,7 @@
       </c>
       <c r="AH16" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.9215686274509802</v>
       </c>
       <c r="AI16" s="3">
         <f t="shared" si="5"/>
@@ -1751,7 +1769,7 @@
     <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1816,7 +1834,7 @@
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1832,12 +1850,8 @@
         <v>0</v>
       </c>
       <c r="M18" s="1"/>
-      <c r="N18" s="1">
-        <v>0</v>
-      </c>
-      <c r="O18" s="1">
-        <v>1</v>
-      </c>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="1"/>
@@ -1855,11 +1869,11 @@
       <c r="AD18" s="1"/>
       <c r="AE18" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF18" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG18" s="1">
         <f t="shared" si="3"/>
@@ -1867,7 +1881,7 @@
       </c>
       <c r="AH18" s="3">
         <f t="shared" si="4"/>
-        <v>3.9215686274509802</v>
+        <v>0</v>
       </c>
       <c r="AI18" s="3">
         <f t="shared" si="5"/>
@@ -1885,7 +1899,7 @@
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1950,7 +1964,7 @@
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1969,7 +1983,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-      <c r="Q20" s="8"/>
+      <c r="Q20" s="6"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
@@ -2015,7 +2029,7 @@
     <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2031,9 +2045,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="1"/>
-      <c r="N21" s="1">
-        <v>0</v>
-      </c>
+      <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="7"/>
@@ -2082,7 +2094,7 @@
     <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2147,7 +2159,7 @@
     <row r="23" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2163,10 +2175,12 @@
         <v>0</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
+      <c r="Q23" s="7"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
@@ -2212,7 +2226,7 @@
     <row r="24" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2275,11 +2289,9 @@
       <c r="AL24" s="4"/>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A25" s="1"/>
       <c r="B25" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2344,7 +2356,7 @@
     <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2360,12 +2372,10 @@
         <v>0</v>
       </c>
       <c r="M26" s="1"/>
-      <c r="N26" s="1">
-        <v>0</v>
-      </c>
+      <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-      <c r="Q26" s="7"/>
+      <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
@@ -3463,7 +3473,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L43" si="7">SUM(C43:K43)</f>
         <v>0</v>
       </c>
       <c r="M43" s="1"/>
@@ -3519,11 +3529,11 @@
         <v>1.5</v>
       </c>
       <c r="AE43" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AE43" si="8">SUM(M43:AD43)</f>
         <v>25.5</v>
       </c>
       <c r="AF43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AF43" si="9">L43+AE43</f>
         <v>25.5</v>
       </c>
       <c r="AG43" s="1">
@@ -3531,18 +3541,18 @@
         <v>25.5</v>
       </c>
       <c r="AH43" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AH43" si="10">(AF43/AG43)*100</f>
         <v>100</v>
       </c>
       <c r="AI43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AI43" si="11">MAX(IF(AH43&gt;=20,2,0),IF(AH43&gt;=40,3,0),IF(AH43&gt;=60,4,0),IF(AH43&gt;=80,5,0))</f>
         <v>5</v>
       </c>
       <c r="AJ43" s="10">
         <v>0</v>
       </c>
       <c r="AK43" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="AK43" si="12">0.8*AI43+0.2*AJ43</f>
         <v>4</v>
       </c>
       <c r="AL43" s="4"/>
@@ -41788,6 +41798,9 @@
       <c r="AL999" s="14"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AL42">
+    <sortCondition descending="1" ref="AF2:AF42"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update achievement. Add students examples.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C687DFD-EC7A-4593-8853-DA1856650187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB8046A-906B-4296-80D7-C72F8DD02ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:AL999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -596,7 +596,9 @@
     <col min="16" max="16" width="5.44140625" customWidth="1"/>
     <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="30" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="30" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="6" bestFit="1" customWidth="1"/>
@@ -1106,7 +1108,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
@@ -1120,11 +1122,11 @@
       <c r="AD7" s="1"/>
       <c r="AE7" s="1">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="AF7" s="1">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="3"/>
@@ -1132,18 +1134,18 @@
       </c>
       <c r="AH7" s="3">
         <f t="shared" si="4"/>
-        <v>17.647058823529413</v>
+        <v>25.490196078431371</v>
       </c>
       <c r="AI7" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ7" s="3">
         <v>0</v>
       </c>
       <c r="AK7" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AL7" s="4"/>
     </row>
@@ -1178,7 +1180,9 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
+      <c r="T8" s="1">
+        <v>4</v>
+      </c>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
@@ -1191,11 +1195,11 @@
       <c r="AD8" s="1"/>
       <c r="AE8" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AF8" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="3"/>
@@ -1203,7 +1207,7 @@
       </c>
       <c r="AH8" s="3">
         <f t="shared" si="4"/>
-        <v>3.9215686274509802</v>
+        <v>19.607843137254903</v>
       </c>
       <c r="AI8" s="3">
         <f t="shared" si="5"/>
@@ -1318,7 +1322,9 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
+      <c r="T10" s="1">
+        <v>2.75</v>
+      </c>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
@@ -1331,11 +1337,11 @@
       <c r="AD10" s="1"/>
       <c r="AE10" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.75</v>
       </c>
       <c r="AF10" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3.75</v>
       </c>
       <c r="AG10" s="1">
         <f t="shared" si="3"/>
@@ -1343,7 +1349,7 @@
       </c>
       <c r="AH10" s="3">
         <f t="shared" si="4"/>
-        <v>3.9215686274509802</v>
+        <v>14.705882352941178</v>
       </c>
       <c r="AI10" s="3">
         <f t="shared" si="5"/>
@@ -1385,7 +1391,9 @@
         <v>0.75</v>
       </c>
       <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
+      <c r="T11" s="1">
+        <v>0.5</v>
+      </c>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
@@ -1398,11 +1406,11 @@
       <c r="AD11" s="1"/>
       <c r="AE11" s="1">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="AF11" s="1">
         <f t="shared" si="2"/>
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="AG11" s="1">
         <f t="shared" si="3"/>
@@ -1410,7 +1418,7 @@
       </c>
       <c r="AH11" s="3">
         <f t="shared" si="4"/>
-        <v>2.9411764705882351</v>
+        <v>4.9019607843137258</v>
       </c>
       <c r="AI11" s="3">
         <f t="shared" si="5"/>

</xml_diff>